<commit_message>
New Version Excel reader added
</commit_message>
<xml_diff>
--- a/EAEmployeeTest/Data/Login.xlsx
+++ b/EAEmployeeTest/Data/Login.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E88E455-03D3-42EF-B1AF-626BC51B5815}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -71,7 +70,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -132,7 +131,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -167,7 +166,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -348,19 +347,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -368,7 +364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>

</xml_diff>